<commit_message>
Half done with project. Graph working for few datasets.
</commit_message>
<xml_diff>
--- a/Backend/Excel/Admissions Data.xlsx
+++ b/Backend/Excel/Admissions Data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bipularyal/Desktop/FISK_IPDES_Proj/Backend/Excel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AFC288A-E684-1E4B-9E19-3B0AC9FB48D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{887A9852-954A-D244-ADD6-AA9C00BCFCB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2000" windowWidth="27640" windowHeight="16940" xr2:uid="{7A2C989B-8DE1-0045-8994-F292EA3A06F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,18 +36,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Year</t>
   </si>
   <si>
-    <t>Number of applicants</t>
+    <t>applicants</t>
   </si>
   <si>
-    <t>Percent admitted</t>
+    <t>percentageAdmitted</t>
   </si>
   <si>
-    <t>Percent admitted who enrolled</t>
+    <t>percEnrolled</t>
+  </si>
+  <si>
+    <t>totalEnrolled</t>
   </si>
 </sst>
 </file>
@@ -413,10 +416,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2F35F74F-DF6B-2343-B327-BBD019815295}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -427,7 +430,7 @@
     <col min="4" max="4" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,8 +443,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>2010</v>
       </c>
@@ -454,8 +460,12 @@
       <c r="D2" s="2">
         <v>0.19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E2">
+        <f>INT(B2*C2*D2)</f>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2011</v>
       </c>
@@ -468,8 +478,12 @@
       <c r="D3" s="2">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E3">
+        <f t="shared" ref="E3:E14" si="0">INT(B3*C3*D3)</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>2012</v>
       </c>
@@ -482,8 +496,12 @@
       <c r="D4" s="2">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <f t="shared" si="0"/>
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>2013</v>
       </c>
@@ -496,8 +514,12 @@
       <c r="D5" s="2">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>2014</v>
       </c>
@@ -510,8 +532,12 @@
       <c r="D6" s="2">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>232</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>2015</v>
       </c>
@@ -524,8 +550,12 @@
       <c r="D7" s="2">
         <v>0.09</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>2016</v>
       </c>
@@ -538,8 +568,12 @@
       <c r="D8" s="2">
         <v>0.04</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <f t="shared" si="0"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>2017</v>
       </c>
@@ -552,8 +586,12 @@
       <c r="D9" s="2">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E9">
+        <f t="shared" si="0"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>2018</v>
       </c>
@@ -566,8 +604,12 @@
       <c r="D10" s="2">
         <v>0.22</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E10">
+        <f t="shared" si="0"/>
+        <v>295</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>2019</v>
       </c>
@@ -580,8 +622,12 @@
       <c r="D11" s="2">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E11">
+        <f t="shared" si="0"/>
+        <v>338</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>2020</v>
       </c>
@@ -594,8 +640,12 @@
       <c r="D12" s="2">
         <v>0.06</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E12">
+        <f t="shared" si="0"/>
+        <v>251</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>2021</v>
       </c>
@@ -608,8 +658,12 @@
       <c r="D13" s="2">
         <v>0.11</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>287</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>2022</v>
       </c>
@@ -621,6 +675,10 @@
       </c>
       <c r="D14" s="2">
         <v>0.06</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="0"/>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>